<commit_message>
complete section4:common stats functions
</commit_message>
<xml_diff>
--- a/homework_workbook/Excel_Homework_Exercises.xlsx
+++ b/homework_workbook/Excel_Homework_Exercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MASTER\Documents\Especializacion\Excel\craft_excel\homework_workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B06A50-C077-4F64-B9CD-F2C7EEEE264C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF13F60-FB18-48BA-A4DC-BAC06F61AB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="709" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="709" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formulas 101" sheetId="19" r:id="rId1"/>
@@ -968,7 +968,7 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1130,9 +1130,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5481,7 +5478,7 @@
         <v>0.35678391959798994</v>
       </c>
       <c r="F4" s="56">
-        <f t="shared" ref="F3:F26" si="1">D4/$B4</f>
+        <f t="shared" ref="F4:F26" si="1">D4/$B4</f>
         <v>9.5477386934673364E-2</v>
       </c>
     </row>
@@ -6063,7 +6060,7 @@
       <c r="B9" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C9" s="66"/>
+      <c r="C9" s="65"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9"/>
@@ -6153,7 +6150,7 @@
     <col min="3" max="3" width="17.42578125" style="43" customWidth="1"/>
     <col min="4" max="5" width="14.85546875" style="43" customWidth="1"/>
     <col min="6" max="6" width="24" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="65" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="64" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -6175,7 +6172,7 @@
       <c r="F1" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="63" t="s">
         <v>131</v>
       </c>
     </row>
@@ -6199,7 +6196,7 @@
       <c r="F2" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="67">
+      <c r="G2" s="66">
         <f>E2/B2</f>
         <v>0.41492265696087355</v>
       </c>
@@ -6224,7 +6221,7 @@
       <c r="F3" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="68">
+      <c r="G3" s="67">
         <f t="shared" ref="G3:G25" si="0">E3/B3</f>
         <v>0.17524916943521596</v>
       </c>
@@ -6250,7 +6247,7 @@
       <c r="F4" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="67">
         <f t="shared" si="0"/>
         <v>0.50411522633744854</v>
       </c>
@@ -6276,7 +6273,7 @@
       <c r="F5" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G5" s="68">
+      <c r="G5" s="67">
         <f t="shared" si="0"/>
         <v>0.52380952380952384</v>
       </c>
@@ -6302,7 +6299,7 @@
       <c r="F6" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G6" s="68">
+      <c r="G6" s="67">
         <f t="shared" si="0"/>
         <v>0.43443132380360472</v>
       </c>
@@ -6328,7 +6325,7 @@
       <c r="F7" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G7" s="68">
+      <c r="G7" s="67">
         <f t="shared" si="0"/>
         <v>0.39156626506024095</v>
       </c>
@@ -6354,7 +6351,7 @@
       <c r="F8" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G8" s="68">
+      <c r="G8" s="67">
         <f t="shared" si="0"/>
         <v>0.57631444614599281</v>
       </c>
@@ -6380,7 +6377,7 @@
       <c r="F9" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G9" s="68">
+      <c r="G9" s="67">
         <f t="shared" si="0"/>
         <v>0.51498929336188437</v>
       </c>
@@ -6406,7 +6403,7 @@
       <c r="F10" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G10" s="68">
+      <c r="G10" s="67">
         <f t="shared" si="0"/>
         <v>0.47848537005163511</v>
       </c>
@@ -6432,7 +6429,7 @@
       <c r="F11" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G11" s="68">
+      <c r="G11" s="67">
         <f t="shared" si="0"/>
         <v>0.3377808988764045</v>
       </c>
@@ -6458,7 +6455,7 @@
       <c r="F12" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G12" s="68">
+      <c r="G12" s="67">
         <f t="shared" si="0"/>
         <v>0.34983766233766234</v>
       </c>
@@ -6484,7 +6481,7 @@
       <c r="F13" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G13" s="68">
+      <c r="G13" s="67">
         <f t="shared" si="0"/>
         <v>0.54775604142692746</v>
       </c>
@@ -6510,7 +6507,7 @@
       <c r="F14" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G14" s="68">
+      <c r="G14" s="67">
         <f t="shared" si="0"/>
         <v>0.5993031358885017</v>
       </c>
@@ -6536,7 +6533,7 @@
       <c r="F15" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G15" s="68">
+      <c r="G15" s="67">
         <f t="shared" si="0"/>
         <v>0.59571045576407511</v>
       </c>
@@ -6562,7 +6559,7 @@
       <c r="F16" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G16" s="68">
+      <c r="G16" s="67">
         <f t="shared" si="0"/>
         <v>0.51458670988654787</v>
       </c>
@@ -6588,7 +6585,7 @@
       <c r="F17" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G17" s="68">
+      <c r="G17" s="67">
         <f t="shared" si="0"/>
         <v>0.40393151553582751</v>
       </c>
@@ -6614,7 +6611,7 @@
       <c r="F18" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G18" s="68">
+      <c r="G18" s="67">
         <f t="shared" si="0"/>
         <v>0.51891074130105896</v>
       </c>
@@ -6640,7 +6637,7 @@
       <c r="F19" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G19" s="68">
+      <c r="G19" s="67">
         <f t="shared" si="0"/>
         <v>0.57448377581120946</v>
       </c>
@@ -6665,7 +6662,7 @@
       <c r="F20" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G20" s="68">
+      <c r="G20" s="67">
         <f t="shared" si="0"/>
         <v>0.47118463180362863</v>
       </c>
@@ -6691,7 +6688,7 @@
       <c r="F21" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G21" s="68">
+      <c r="G21" s="67">
         <f t="shared" si="0"/>
         <v>0.60243407707910746</v>
       </c>
@@ -6716,7 +6713,7 @@
       <c r="F22" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G22" s="68">
+      <c r="G22" s="67">
         <f t="shared" si="0"/>
         <v>0.36644364384971695</v>
       </c>
@@ -6742,7 +6739,7 @@
       <c r="F23" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G23" s="68">
+      <c r="G23" s="67">
         <f t="shared" si="0"/>
         <v>0.54501385041551242</v>
       </c>
@@ -6768,7 +6765,7 @@
       <c r="F24" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G24" s="68">
+      <c r="G24" s="67">
         <f t="shared" si="0"/>
         <v>0.4105827193569993</v>
       </c>
@@ -6794,7 +6791,7 @@
       <c r="F25" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G25" s="68">
+      <c r="G25" s="67">
         <f t="shared" si="0"/>
         <v>0.66628308400460301</v>
       </c>
@@ -6812,9 +6809,7 @@
   </sheetPr>
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6849,19 +6844,19 @@
       <c r="E1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="68" t="s">
         <v>206</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="68" t="s">
         <v>207</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="68" t="s">
         <v>208</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="68" t="s">
         <v>209</v>
       </c>
-      <c r="K1" s="69" t="s">
+      <c r="K1" s="68" t="s">
         <v>210</v>
       </c>
     </row>
@@ -6889,7 +6884,7 @@
       <c r="M2" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="N2" s="66"/>
+      <c r="N2" s="65"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -6934,10 +6929,10 @@
       <c r="I4" s="2"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
-      <c r="M4" s="69" t="s">
+      <c r="M4" s="68" t="s">
         <v>208</v>
       </c>
-      <c r="N4" s="69" t="s">
+      <c r="N4" s="68" t="s">
         <v>210</v>
       </c>
     </row>
@@ -6981,7 +6976,7 @@
       <c r="E6" s="8">
         <v>10283</v>
       </c>
-      <c r="G6" s="70"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="8"/>
@@ -7005,7 +7000,7 @@
       <c r="E7" s="8">
         <v>15332</v>
       </c>
-      <c r="G7" s="70"/>
+      <c r="G7" s="69"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="8"/>
@@ -7035,7 +7030,7 @@
       <c r="M8" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="N8" s="71" t="s">
+      <c r="N8" s="70" t="s">
         <v>212</v>
       </c>
     </row>
@@ -7082,19 +7077,19 @@
       <c r="I10" s="2"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="M10" s="69" t="s">
+      <c r="M10" s="68" t="s">
         <v>206</v>
       </c>
-      <c r="N10" s="69" t="s">
+      <c r="N10" s="68" t="s">
         <v>207</v>
       </c>
-      <c r="O10" s="69" t="s">
+      <c r="O10" s="68" t="s">
         <v>208</v>
       </c>
-      <c r="P10" s="69" t="s">
+      <c r="P10" s="68" t="s">
         <v>209</v>
       </c>
-      <c r="Q10" s="69" t="s">
+      <c r="Q10" s="68" t="s">
         <v>210</v>
       </c>
     </row>
@@ -7251,10 +7246,10 @@
       <c r="K16" s="8"/>
     </row>
     <row r="17" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M17" s="69" t="s">
+      <c r="M17" s="68" t="s">
         <v>207</v>
       </c>
-      <c r="N17" s="69" t="s">
+      <c r="N17" s="68" t="s">
         <v>232</v>
       </c>
     </row>
@@ -7289,7 +7284,7 @@
   </sheetPr>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -7403,7 +7398,7 @@
         <v>OUTLIER</v>
       </c>
       <c r="G4" s="55" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C4&gt;95,IF(B4="M","Male achiever","Female achiever"),"None")</f>
         <v>Female achiever</v>
       </c>
     </row>
@@ -7744,7 +7739,9 @@
   </sheetPr>
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7870,7 +7867,10 @@
       <c r="E5" s="8">
         <v>3072</v>
       </c>
-      <c r="H5" s="48"/>
+      <c r="H5" s="48">
+        <f>SUMIF(A2:A70,H2,D2:D70)</f>
+        <v>620</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -7934,9 +7934,18 @@
       <c r="G8" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="H8" s="48"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="48"/>
+      <c r="H8" s="48">
+        <f>SUMIFS(D$2:D$70,$C$2:$C$70,$G8,$A$2:$A$70,$H$2)</f>
+        <v>166</v>
+      </c>
+      <c r="I8" s="48">
+        <f t="shared" ref="I8:J10" si="0">SUMIFS(E$2:E$70,$C$2:$C$70,$G8,$A$2:$A$70,$H$2)</f>
+        <v>10015</v>
+      </c>
+      <c r="J8" s="48">
+        <f>COUNTIFS($C$2:$C$70,$G8,$A$2:$A$70,$H$2)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -7957,9 +7966,18 @@
       <c r="G9" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="48"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="48"/>
+      <c r="H9" s="48">
+        <f t="shared" ref="H9:H10" si="1">SUMIFS(D$2:D$70,$C$2:$C$70,$G9,$A$2:$A$70,$H$2)</f>
+        <v>372</v>
+      </c>
+      <c r="I9" s="48">
+        <f t="shared" si="0"/>
+        <v>42628</v>
+      </c>
+      <c r="J9" s="48">
+        <f t="shared" ref="J9:J10" si="2">COUNTIFS($C$2:$C$70,$G9,$A$2:$A$70,$H$2)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -7980,9 +7998,18 @@
       <c r="G10" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="48"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="48"/>
+      <c r="H10" s="48">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="I10" s="48">
+        <f t="shared" si="0"/>
+        <v>6300</v>
+      </c>
+      <c r="J10" s="48">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -14903,7 +14930,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" style="63" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="62" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
@@ -14913,7 +14940,7 @@
       <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="61" t="s">
         <v>204</v>
       </c>
       <c r="C1" s="21" t="s">
@@ -14939,7 +14966,7 @@
       <c r="F2" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="G2" s="60"/>
+      <c r="G2" s="59"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -14957,7 +14984,7 @@
       <c r="F3" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="G3" s="60"/>
+      <c r="G3" s="59"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
@@ -14989,7 +15016,7 @@
       <c r="F5" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="G5" s="61"/>
+      <c r="G5" s="60"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">

</xml_diff>